<commit_message>
attack speed  + anim speed player
</commit_message>
<xml_diff>
--- a/Assets/8_Data/0_PlayerData.xlsx
+++ b/Assets/8_Data/0_PlayerData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ba Sumo\Documents\Projects\Evolver\Assets\8_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unity_Game\Evolver\Assets\8_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -595,7 +595,7 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,19 +674,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>50</v>
+        <v>11111</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="G3">
         <v>7</v>
@@ -712,10 +712,10 @@
         <v>2</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4">
         <v>7</v>
@@ -741,10 +741,10 @@
         <v>3</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
         <v>7</v>
@@ -770,10 +770,10 @@
         <v>4</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6">
         <v>7</v>

</xml_diff>